<commit_message>
Inicie mecanismo de exportacion e importacion
</commit_message>
<xml_diff>
--- a/resguardo/mecanismo.xlsx
+++ b/resguardo/mecanismo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\TECNICATURA\Laboratorio ll\TP2\Booking\backups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\TECNICATURA\Laboratorio ll\TP2\Booking\resguardo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>usuarios</t>
   </si>
@@ -131,27 +131,12 @@
     <t>tipo</t>
   </si>
   <si>
-    <t>int (1, 2, 3)</t>
-  </si>
-  <si>
     <t>int (0, 1)</t>
   </si>
   <si>
     <t>minimos_categoria</t>
   </si>
   <si>
-    <t>imágenes</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>añadir imágenes</t>
-  </si>
-  <si>
-    <t>servicios</t>
-  </si>
-  <si>
     <t>ac</t>
   </si>
   <si>
@@ -173,9 +158,6 @@
     <t>desayuno</t>
   </si>
   <si>
-    <t>añadir servicios</t>
-  </si>
-  <si>
     <t>Crear reservas</t>
   </si>
   <si>
@@ -207,6 +189,24 @@
   </si>
   <si>
     <t>int (pk)</t>
+  </si>
+  <si>
+    <t>eliminada</t>
+  </si>
+  <si>
+    <t>bool = false</t>
+  </si>
+  <si>
+    <t>imagen_1</t>
+  </si>
+  <si>
+    <t>imagen_2</t>
+  </si>
+  <si>
+    <t>int (0,1,2)</t>
+  </si>
+  <si>
+    <t>int = -1</t>
   </si>
 </sst>
 </file>
@@ -238,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -320,7 +326,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,246 +351,205 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>688074</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>176579</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>690210</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>5340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Conector recto de flecha 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3428343" y="557579"/>
+          <a:ext cx="2136" cy="590761"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>550251</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>162903</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>656782</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>169844</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Conector recto de flecha 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3290520" y="2067903"/>
+          <a:ext cx="1476666" cy="578441"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>652096</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>146540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>534865</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Conector recto de flecha 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3392365" y="4337540"/>
+          <a:ext cx="1252904" cy="608133"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>652096</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>647703</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>548054</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>174382</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="54" name="Grupo 53"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="2247900" y="476250"/>
-          <a:ext cx="2752728" cy="5238751"/>
-          <a:chOff x="2247900" y="476250"/>
-          <a:chExt cx="2752728" cy="5238751"/>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector recto de flecha 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3392365" y="2842846"/>
+          <a:ext cx="2636227" cy="2094036"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="32" name="Conector recto de flecha 31"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="2257425" y="476250"/>
-            <a:ext cx="1419225" cy="666750"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="35" name="Conector recto de flecha 34"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="2247900" y="1990725"/>
-            <a:ext cx="1428750" cy="676275"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="36" name="Conector recto de flecha 35"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="2276446" y="2744011"/>
-            <a:ext cx="1200180" cy="694514"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="37" name="Conector recto de flecha 36"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="2286001" y="2733676"/>
-            <a:ext cx="1714499" cy="1457324"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="39" name="Conector recto de flecha 38"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="2247900" y="5038725"/>
-            <a:ext cx="1428750" cy="676275"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="40" name="Conector recto de flecha 39"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="2292641" y="2727798"/>
-            <a:ext cx="2707987" cy="2987203"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -851,21 +818,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="11" width="19.85546875" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" customWidth="1"/>
+    <col min="1" max="21" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -878,8 +842,17 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -892,9 +865,18 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -910,25 +892,38 @@
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="6" t="s">
-        <v>51</v>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -936,128 +931,177 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="K7" s="8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1069,9 +1113,18 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1087,20 +1140,31 @@
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
@@ -1111,15 +1175,26 @@
       <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1131,9 +1206,18 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1145,9 +1229,18 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1248,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>34</v>
@@ -1176,25 +1269,52 @@
         <v>28</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="P15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U15" s="4"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1210,11 +1330,38 @@
         <v>29</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U16" s="4"/>
+    </row>
+    <row r="17" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1227,8 +1374,17 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1241,66 +1397,114 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="F20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+    </row>
+    <row r="21" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1313,86 +1517,118 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1405,178 +1641,15 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-    </row>
-    <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finalice sistema de exportacion
</commit_message>
<xml_diff>
--- a/resguardo/mecanismo.xlsx
+++ b/resguardo/mecanismo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
   <si>
     <t>usuarios</t>
   </si>
@@ -65,9 +65,6 @@
     <t>dni</t>
   </si>
   <si>
-    <t>clientes</t>
-  </si>
-  <si>
     <t>sesiones</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>id_cliente</t>
-  </si>
-  <si>
     <t>long</t>
   </si>
   <si>
@@ -116,18 +110,6 @@
     <t>double</t>
   </si>
   <si>
-    <t>Crear usuarios</t>
-  </si>
-  <si>
-    <t>Crear sesiones</t>
-  </si>
-  <si>
-    <t>Crear propietarios</t>
-  </si>
-  <si>
-    <t>Crear propiedades</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
@@ -158,18 +140,6 @@
     <t>desayuno</t>
   </si>
   <si>
-    <t>Crear reservas</t>
-  </si>
-  <si>
-    <t>Pasos</t>
-  </si>
-  <si>
-    <t>añadir a propiedad</t>
-  </si>
-  <si>
-    <t>Crear clientes</t>
-  </si>
-  <si>
     <t>id_propietario</t>
   </si>
   <si>
@@ -179,12 +149,6 @@
     <t>activa</t>
   </si>
   <si>
-    <t>añadir a usuarios</t>
-  </si>
-  <si>
-    <t>añadir a propietarios</t>
-  </si>
-  <si>
     <t>int (fk)</t>
   </si>
   <si>
@@ -207,6 +171,18 @@
   </si>
   <si>
     <t>int = -1</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Servicios</t>
+  </si>
+  <si>
+    <t>crear/guardar</t>
+  </si>
+  <si>
+    <t>localidades</t>
   </si>
 </sst>
 </file>
@@ -238,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,8 +251,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -312,11 +294,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -328,7 +347,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,15 +379,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>688074</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>176579</xdr:rowOff>
+      <xdr:colOff>280635</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>690210</xdr:colOff>
+      <xdr:colOff>280635</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>5340</xdr:rowOff>
+      <xdr:rowOff>5341</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -367,9 +395,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3428343" y="557579"/>
-          <a:ext cx="2136" cy="590761"/>
+        <a:xfrm flipV="1">
+          <a:off x="1585560" y="781050"/>
+          <a:ext cx="0" cy="367291"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -402,15 +430,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>550251</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>162903</xdr:rowOff>
+      <xdr:colOff>274840</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>656782</xdr:colOff>
+      <xdr:colOff>285308</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>169844</xdr:rowOff>
+      <xdr:rowOff>169845</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -419,8 +447,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3290520" y="2067903"/>
-          <a:ext cx="1476666" cy="578441"/>
+          <a:off x="1579765" y="2286000"/>
+          <a:ext cx="515293" cy="360345"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -453,76 +481,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>652096</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>146540</xdr:rowOff>
+      <xdr:colOff>274840</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>534865</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>183173</xdr:rowOff>
+      <xdr:colOff>294833</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>169845</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Conector recto de flecha 11"/>
+        <xdr:cNvPr id="10" name="Conector recto de flecha 9"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3392365" y="4337540"/>
-          <a:ext cx="1252904" cy="608133"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="00B050"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>652096</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>175846</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>548054</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>174382</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Conector recto de flecha 13"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3392365" y="2842846"/>
-          <a:ext cx="2636227" cy="2094036"/>
+          <a:off x="1579765" y="3048000"/>
+          <a:ext cx="524818" cy="360345"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -818,15 +795,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="21" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -881,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -893,16 +889,16 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -920,10 +916,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -938,10 +934,10 @@
         <v>9</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -963,11 +959,9 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="8" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -990,10 +984,10 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -1008,7 +1002,7 @@
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1023,11 +1017,9 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="J7" s="4"/>
       <c r="K7" s="8" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1046,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1058,10 +1050,10 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1083,11 +1075,9 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="J9" s="4"/>
       <c r="K9" s="8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -1126,22 +1116,22 @@
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1164,7 +1154,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
@@ -1173,10 +1163,10 @@
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1198,7 +1188,7 @@
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1231,72 +1221,74 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="O14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="13"/>
       <c r="U14" s="4"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="J15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="U15" s="4"/>
     </row>
@@ -1306,15 +1298,15 @@
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1327,10 +1319,10 @@
         <v>9</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>9</v>
@@ -1339,30 +1331,30 @@
         <v>9</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="U16" s="4"/>
     </row>
     <row r="17" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1385,7 +1377,7 @@
       <c r="U17" s="4"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1393,11 +1385,13 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="I18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -1408,33 +1402,43 @@
       <c r="U18" s="4"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="J19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -1445,33 +1449,43 @@
       <c r="U19" s="4"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="K20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -1484,7 +1498,7 @@
     <row r="21" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1504,15 +1518,15 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1527,32 +1541,16 @@
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -1566,32 +1564,16 @@
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1651,7 +1633,149 @@
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
     </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="O14:T14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Inicie y termine mecanismo de importacion
</commit_message>
<xml_diff>
--- a/resguardo/mecanismo.xlsx
+++ b/resguardo/mecanismo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
   <si>
     <t>usuarios</t>
   </si>
@@ -38,9 +38,6 @@
     <t>salida</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
     <t>categoria</t>
   </si>
   <si>
@@ -183,6 +180,30 @@
   </si>
   <si>
     <t>localidades</t>
+  </si>
+  <si>
+    <t>primary keys</t>
+  </si>
+  <si>
+    <t>primarykeys</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>sesion</t>
+  </si>
+  <si>
+    <t>propietario</t>
+  </si>
+  <si>
+    <t>propiedad</t>
+  </si>
+  <si>
+    <t>reserva</t>
+  </si>
+  <si>
+    <t>id_usuario</t>
   </si>
 </sst>
 </file>
@@ -214,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +275,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -347,6 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -356,13 +384,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -378,15 +415,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>280635</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>280635</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>5341</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -429,15 +466,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>274840</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>285308</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>169845</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -480,15 +517,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>274840</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>294833</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>169845</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -795,63 +832,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" customWidth="1"/>
+    <col min="1" max="2" width="2" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C1" s="17">
+        <v>0</v>
+      </c>
+      <c r="D1" s="17">
+        <v>1</v>
+      </c>
+      <c r="E1" s="17">
+        <v>2</v>
+      </c>
+      <c r="F1" s="17">
+        <v>3</v>
+      </c>
+      <c r="G1" s="17">
+        <v>4</v>
+      </c>
+      <c r="H1" s="17">
+        <v>5</v>
+      </c>
+      <c r="I1" s="17">
+        <v>6</v>
+      </c>
+      <c r="J1" s="17">
+        <v>7</v>
+      </c>
+      <c r="K1" s="17">
+        <v>8</v>
+      </c>
+      <c r="L1" s="17">
+        <v>9</v>
+      </c>
+      <c r="M1" s="17">
+        <v>10</v>
+      </c>
+      <c r="N1" s="17">
+        <v>11</v>
+      </c>
+      <c r="O1" s="17">
+        <v>12</v>
+      </c>
+      <c r="P1" s="17">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="17">
+        <v>14</v>
+      </c>
+      <c r="R1" s="17">
+        <v>15</v>
+      </c>
+      <c r="S1" s="17">
+        <v>16</v>
+      </c>
+      <c r="T1" s="17">
+        <v>17</v>
+      </c>
+      <c r="U1" s="17">
+        <v>18</v>
+      </c>
+      <c r="V1" s="4"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -870,35 +945,30 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="4"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -909,35 +979,30 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -948,9 +1013,10 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="V4" s="4"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -960,9 +1026,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -973,9 +1037,10 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -985,9 +1050,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -998,30 +1061,37 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" s="4"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B7" s="15"/>
       <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J7" s="4"/>
-      <c r="K7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1031,30 +1101,37 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" s="4"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1064,9 +1141,10 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="V8" s="4"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1076,10 +1154,10 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1089,9 +1167,10 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1102,7 +1181,9 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="L10" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1112,32 +1193,31 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" s="4"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="L11" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1147,32 +1227,31 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" s="4"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="L12" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1182,20 +1261,23 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="V12" s="4"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="L13" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1205,9 +1287,10 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="V13" s="4"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1218,153 +1301,104 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="L14" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="13"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
       <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" s="4"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
       <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" s="4"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
       <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="V16" s="4"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -1375,9 +1409,10 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="V17" s="4"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1385,129 +1420,160 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="13"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="4"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V19" s="4"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="I20" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V20" s="4"/>
+    </row>
+    <row r="21" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1517,22 +1583,25 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="4"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="J22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="14"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -1540,22 +1609,47 @@
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
+      <c r="V22" s="4"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -1563,40 +1657,66 @@
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="V23" s="4"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
+      <c r="R24" s="9"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="4"/>
+    </row>
+    <row r="25" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -1609,17 +1729,18 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="4"/>
+    </row>
+    <row r="26" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -1632,17 +1753,22 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="V26" s="4"/>
+    </row>
+    <row r="27" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1655,17 +1781,22 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="V27" s="4"/>
+    </row>
+    <row r="28" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1678,17 +1809,18 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="4"/>
+    </row>
+    <row r="29" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -1701,8 +1833,9 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="4"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1724,57 +1857,12 @@
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
+      <c r="V30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="O14:T14"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="P18:U18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>